<commit_message>
update gait results for testing. 1 IC values shifted by 1 index, 1-2 delta h values updated
</commit_message>
<xml_diff>
--- a/tests/gait/data/manual_gait_results_apcwt.xlsx
+++ b/tests/gait/data/manual_gait_results_apcwt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasadamowicz/Documents/Packages/scikit-digital-health/tests/gait/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76059E6-5BAA-9641-A85C-10A0DF0A7DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAB0BD2-E488-AD42-9225-BA11AA6A73D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="31720" windowHeight="24660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31620" yWindow="2020" windowWidth="31720" windowHeight="24660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tmp" sheetId="1" r:id="rId1"/>
@@ -1022,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:O81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1166,13 +1166,13 @@
         <v>-1</v>
       </c>
       <c r="M2">
-        <v>0.1615208812585911</v>
+        <v>0.16152088125859149</v>
       </c>
       <c r="N2">
-        <v>4.0444692655927518E-2</v>
+        <v>4.0444692655927539E-2</v>
       </c>
       <c r="O2">
-        <v>2.4586382323534502E-2</v>
+        <v>2.4586382323534491E-2</v>
       </c>
       <c r="P2">
         <v>0.99639999999999995</v>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="AD2">
         <f>2 * SQRT(2 * P2 * N2 - N2 * N2) + 2 * SQRT(2 * AC2 * O2 - O2 * O2)</f>
-        <v>0.85151243926887421</v>
+        <v>0.85151243926887443</v>
       </c>
       <c r="AE2">
         <f>AD2+AD3</f>
@@ -1283,7 +1283,7 @@
         <v>-1</v>
       </c>
       <c r="M3">
-        <v>0.14485628024775679</v>
+        <v>0.1448562802477571</v>
       </c>
       <c r="N3">
         <v>3.7534385891120382E-2</v>
@@ -1400,7 +1400,7 @@
         <v>-1</v>
       </c>
       <c r="M4">
-        <v>0.129850131922465</v>
+        <v>0.12985013192246531</v>
       </c>
       <c r="N4">
         <v>3.4236755912058402E-2</v>
@@ -1469,11 +1469,11 @@
       </c>
       <c r="AE4">
         <f t="shared" si="16"/>
-        <v>1.4434768745886017</v>
+        <v>1.4434768745886015</v>
       </c>
       <c r="AF4">
         <f t="shared" si="17"/>
-        <v>1.3122517041714561</v>
+        <v>1.3122517041714559</v>
       </c>
       <c r="AG4">
         <f t="shared" si="18"/>
@@ -1517,13 +1517,13 @@
         <v>-1</v>
       </c>
       <c r="M5">
-        <v>0.1088103625182866</v>
+        <v>0.1088103625182868</v>
       </c>
       <c r="N5">
-        <v>3.5193641570658053E-2</v>
+        <v>3.519364157065806E-2</v>
       </c>
       <c r="O5">
-        <v>9.5700225898245669E-3</v>
+        <v>9.5700225898245651E-3</v>
       </c>
       <c r="P5">
         <v>0.99639999999999995</v>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="AD5">
         <f t="shared" si="15"/>
-        <v>0.70716383288043694</v>
+        <v>0.70716383288043683</v>
       </c>
       <c r="AE5">
         <f t="shared" si="16"/>
@@ -1634,7 +1634,7 @@
         <v>-1</v>
       </c>
       <c r="M6">
-        <v>0.13941298892198731</v>
+        <v>0.1394129889219877</v>
       </c>
       <c r="N6">
         <v>3.5742306315753709E-2</v>
@@ -1703,11 +1703,11 @@
       </c>
       <c r="AE6">
         <f t="shared" si="16"/>
-        <v>1.5784700938596896</v>
+        <v>1.5784700938596898</v>
       </c>
       <c r="AF6">
         <f t="shared" si="17"/>
-        <v>1.384622889350605</v>
+        <v>1.3846228893506052</v>
       </c>
       <c r="AG6">
         <f t="shared" si="18"/>
@@ -1751,10 +1751,10 @@
         <v>-1</v>
       </c>
       <c r="M7">
-        <v>0.13469530687146511</v>
+        <v>0.13469530687146539</v>
       </c>
       <c r="N7">
-        <v>4.5841247026411923E-2</v>
+        <v>4.5841247026411937E-2</v>
       </c>
       <c r="O7">
         <v>1.4228206833498279E-2</v>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="AD7">
         <f t="shared" si="15"/>
-        <v>0.81906807488542277</v>
+        <v>0.81906807488542288</v>
       </c>
       <c r="AE7">
         <f t="shared" si="16"/>
@@ -1868,13 +1868,13 @@
         <v>-1</v>
       </c>
       <c r="M8">
-        <v>0.13223582941588791</v>
+        <v>0.13223582941588821</v>
       </c>
       <c r="N8">
         <v>3.7918631866738613E-2</v>
       </c>
       <c r="O8">
-        <v>1.1488261306114911E-2</v>
+        <v>1.14882613061149E-2</v>
       </c>
       <c r="P8">
         <v>0.99639999999999995</v>
@@ -1933,15 +1933,15 @@
       </c>
       <c r="AD8">
         <f t="shared" si="15"/>
-        <v>0.74393546248284514</v>
+        <v>0.74393546248284503</v>
       </c>
       <c r="AE8">
         <f t="shared" si="16"/>
-        <v>1.4915069551392484</v>
+        <v>1.4915069551392479</v>
       </c>
       <c r="AF8">
         <f t="shared" si="17"/>
-        <v>1.4070820331502343</v>
+        <v>1.4070820331502338</v>
       </c>
       <c r="AG8">
         <f t="shared" si="18"/>
@@ -1985,10 +1985,10 @@
         <v>-1</v>
       </c>
       <c r="M9">
-        <v>0.12854214528226671</v>
+        <v>0.12854214528226701</v>
       </c>
       <c r="N9">
-        <v>3.6866399990195677E-2</v>
+        <v>3.6866399990195663E-2</v>
       </c>
       <c r="O9">
         <v>1.2822572196919121E-2</v>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="AD9">
         <f t="shared" si="15"/>
-        <v>0.7475714926564031</v>
+        <v>0.74757149265640299</v>
       </c>
       <c r="AE9">
         <f t="shared" si="16"/>
@@ -2102,13 +2102,13 @@
         <v>-1</v>
       </c>
       <c r="M10">
-        <v>0.15394091250172171</v>
+        <v>0.15394091250172229</v>
       </c>
       <c r="N10">
-        <v>4.1785039969474427E-2</v>
+        <v>4.1785039969474413E-2</v>
       </c>
       <c r="O10">
-        <v>1.7212581888582129E-2</v>
+        <v>1.721258188858214E-2</v>
       </c>
       <c r="P10">
         <v>0.99639999999999995</v>
@@ -2171,11 +2171,11 @@
       </c>
       <c r="AE10">
         <f t="shared" si="16"/>
-        <v>1.6064046575486515</v>
+        <v>1.6064046575486512</v>
       </c>
       <c r="AF10">
         <f t="shared" si="17"/>
-        <v>1.487411719952455</v>
+        <v>1.4874117199524548</v>
       </c>
       <c r="AG10">
         <f t="shared" si="18"/>
@@ -2219,13 +2219,13 @@
         <v>-1</v>
       </c>
       <c r="M11">
-        <v>0.13138453098173289</v>
+        <v>0.13138453098173319</v>
       </c>
       <c r="N11">
         <v>4.2599275094354121E-2</v>
       </c>
       <c r="O11">
-        <v>1.3462012978144181E-2</v>
+        <v>1.346201297814417E-2</v>
       </c>
       <c r="P11">
         <v>0.99639999999999995</v>
@@ -2284,7 +2284,7 @@
       </c>
       <c r="AD11">
         <f t="shared" si="15"/>
-        <v>0.79207933113626916</v>
+        <v>0.79207933113626905</v>
       </c>
       <c r="AE11">
         <f t="shared" si="16"/>
@@ -2336,13 +2336,13 @@
         <v>-1</v>
       </c>
       <c r="M12">
-        <v>0.15172997034203001</v>
+        <v>0.1517299703420304</v>
       </c>
       <c r="N12">
         <v>4.2502377547009439E-2</v>
       </c>
       <c r="O12">
-        <v>1.6581251183924541E-2</v>
+        <v>1.6581251183924551E-2</v>
       </c>
       <c r="P12">
         <v>0.99639999999999995</v>
@@ -2401,15 +2401,15 @@
       </c>
       <c r="AD12">
         <f t="shared" si="15"/>
-        <v>0.81468466967491937</v>
+        <v>0.81468466967491948</v>
       </c>
       <c r="AE12">
         <f t="shared" si="16"/>
-        <v>1.6190690776292995</v>
+        <v>1.6190690776292997</v>
       </c>
       <c r="AF12">
         <f t="shared" si="17"/>
-        <v>1.5567971900281725</v>
+        <v>1.5567971900281727</v>
       </c>
       <c r="AG12">
         <f t="shared" si="18"/>
@@ -2453,13 +2453,13 @@
         <v>-1</v>
       </c>
       <c r="M13">
-        <v>0.14895689644147031</v>
+        <v>0.1489568964414707</v>
       </c>
       <c r="N13">
-        <v>3.9187498818060162E-2</v>
+        <v>3.9187498818060197E-2</v>
       </c>
       <c r="O13">
-        <v>1.834730393328645E-2</v>
+        <v>1.834730393328643E-2</v>
       </c>
       <c r="P13">
         <v>0.99639999999999995</v>
@@ -2570,13 +2570,13 @@
         <v>-1</v>
       </c>
       <c r="M14">
-        <v>0.1497690638262055</v>
+        <v>0.14976906382620611</v>
       </c>
       <c r="N14">
-        <v>4.9905486260836837E-2</v>
+        <v>4.9905486260836851E-2</v>
       </c>
       <c r="O14">
-        <v>2.5690096816687491E-2</v>
+        <v>2.569009681668747E-2</v>
       </c>
       <c r="P14">
         <v>0.99639999999999995</v>
@@ -2687,13 +2687,13 @@
         <v>-1</v>
       </c>
       <c r="M15">
-        <v>0.14038350571610711</v>
+        <v>0.1403835057161075</v>
       </c>
       <c r="N15">
-        <v>3.965315968068716E-2</v>
+        <v>3.9653159680687187E-2</v>
       </c>
       <c r="O15">
-        <v>1.7929802554382389E-2</v>
+        <v>1.7929802554382371E-2</v>
       </c>
       <c r="P15">
         <v>0.99639999999999995</v>
@@ -2804,10 +2804,10 @@
         <v>-1</v>
       </c>
       <c r="M16">
-        <v>0.1568803917839966</v>
+        <v>0.15688039178399751</v>
       </c>
       <c r="N16">
-        <v>4.9000594673546859E-2</v>
+        <v>4.9000594673546873E-2</v>
       </c>
       <c r="O16">
         <v>2.2666845276049639E-2</v>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="AD16">
         <f t="shared" si="15"/>
-        <v>0.89553258242361999</v>
+        <v>0.8955325824236201</v>
       </c>
       <c r="AE16">
         <f t="shared" si="16"/>
@@ -2921,10 +2921,10 @@
         <v>-1</v>
       </c>
       <c r="M17">
-        <v>0.13460397609291</v>
+        <v>0.13460397609291039</v>
       </c>
       <c r="N17">
-        <v>3.1932499335860211E-2</v>
+        <v>3.1932499335860197E-2</v>
       </c>
       <c r="O17">
         <v>1.103432621850301E-2</v>
@@ -2986,15 +2986,15 @@
       </c>
       <c r="AD17">
         <f t="shared" si="15"/>
-        <v>0.69594534078835879</v>
+        <v>0.69594534078835868</v>
       </c>
       <c r="AE17">
         <f t="shared" si="16"/>
-        <v>1.6177884493532422</v>
+        <v>1.617788449353242</v>
       </c>
       <c r="AF17">
         <f t="shared" si="17"/>
-        <v>1.4191126748712652</v>
+        <v>1.419112674871265</v>
       </c>
       <c r="AG17">
         <f t="shared" si="18"/>
@@ -3038,13 +3038,13 @@
         <v>-1</v>
       </c>
       <c r="M18">
-        <v>0.1747044984542532</v>
+        <v>0.17470449845425409</v>
       </c>
       <c r="N18">
-        <v>4.9572305599925301E-2</v>
+        <v>4.9572305599925273E-2</v>
       </c>
       <c r="O18">
-        <v>2.6659788613929161E-2</v>
+        <v>2.6659788613929172E-2</v>
       </c>
       <c r="P18">
         <v>0.99639999999999995</v>
@@ -3103,15 +3103,15 @@
       </c>
       <c r="AD18">
         <f t="shared" si="15"/>
-        <v>0.9218431085648835</v>
+        <v>0.92184310856488327</v>
       </c>
       <c r="AE18">
         <f t="shared" si="16"/>
-        <v>1.6138628093002028</v>
+        <v>1.6138628093002025</v>
       </c>
       <c r="AF18">
         <f t="shared" si="17"/>
-        <v>1.3228383682788547</v>
+        <v>1.3228383682788545</v>
       </c>
       <c r="AG18">
         <f t="shared" si="18"/>
@@ -3155,13 +3155,13 @@
         <v>-1</v>
       </c>
       <c r="M19">
-        <v>0.14311826857882839</v>
+        <v>0.1431182685788292</v>
       </c>
       <c r="N19">
         <v>3.3299859666551752E-2</v>
       </c>
       <c r="O19">
-        <v>9.4565401871256616E-3</v>
+        <v>9.4565401871256564E-3</v>
       </c>
       <c r="P19">
         <v>0.99639999999999995</v>
@@ -3224,11 +3224,11 @@
       </c>
       <c r="AE19">
         <f t="shared" si="16"/>
-        <v>1.3581651086128801</v>
+        <v>1.3581651086128803</v>
       </c>
       <c r="AF19">
         <f t="shared" si="17"/>
-        <v>1.1913729022920001</v>
+        <v>1.1913729022920003</v>
       </c>
       <c r="AG19">
         <f t="shared" si="18"/>
@@ -3272,10 +3272,10 @@
         <v>-1</v>
       </c>
       <c r="M20">
-        <v>0.1028067010714505</v>
+        <v>0.102806701071451</v>
       </c>
       <c r="N20">
-        <v>3.2349951610360472E-2</v>
+        <v>3.2349951610360493E-2</v>
       </c>
       <c r="O20">
         <v>7.5924926273745778E-3</v>
@@ -3337,15 +3337,15 @@
       </c>
       <c r="AD20">
         <f t="shared" si="15"/>
-        <v>0.66614540787756094</v>
+        <v>0.66614540787756105</v>
       </c>
       <c r="AE20">
         <f t="shared" si="16"/>
-        <v>1.437556993877058</v>
+        <v>1.4375569938770583</v>
       </c>
       <c r="AF20">
         <f t="shared" si="17"/>
-        <v>1.306869994433689</v>
+        <v>1.3068699944336892</v>
       </c>
       <c r="AG20">
         <f t="shared" si="18"/>
@@ -3389,10 +3389,10 @@
         <v>-1</v>
       </c>
       <c r="M21">
-        <v>0.1282558248272147</v>
+        <v>0.1282558248272152</v>
       </c>
       <c r="N21">
-        <v>4.082948696499742E-2</v>
+        <v>4.0829486964997407E-2</v>
       </c>
       <c r="O21">
         <v>1.2367247420086569E-2</v>
@@ -3458,11 +3458,11 @@
       </c>
       <c r="AE21">
         <f t="shared" si="16"/>
-        <v>1.4737103068247082</v>
+        <v>1.4737103068247084</v>
       </c>
       <c r="AF21">
         <f t="shared" si="17"/>
-        <v>1.3397366425679165</v>
+        <v>1.3397366425679167</v>
       </c>
       <c r="AG21">
         <f t="shared" si="18"/>
@@ -3506,13 +3506,13 @@
         <v>-1</v>
       </c>
       <c r="M22">
-        <v>0.11374240877908511</v>
+        <v>0.1137424087790857</v>
       </c>
       <c r="N22">
-        <v>3.3900107373042929E-2</v>
+        <v>3.3900107373042922E-2</v>
       </c>
       <c r="O22">
-        <v>1.0076245322832821E-2</v>
+        <v>1.0076245322832829E-2</v>
       </c>
       <c r="P22">
         <v>0.99639999999999995</v>
@@ -3571,15 +3571,15 @@
       </c>
       <c r="AD22">
         <f t="shared" si="15"/>
-        <v>0.70229872082521105</v>
+        <v>0.70229872082521116</v>
       </c>
       <c r="AE22">
         <f t="shared" si="16"/>
-        <v>1.4326926028124412</v>
+        <v>1.4326926028124414</v>
       </c>
       <c r="AF22">
         <f t="shared" si="17"/>
-        <v>1.3265672248263343</v>
+        <v>1.3265672248263345</v>
       </c>
       <c r="AG22">
         <f t="shared" si="18"/>
@@ -3623,10 +3623,10 @@
         <v>-1</v>
       </c>
       <c r="M23">
-        <v>0.1248677809592874</v>
+        <v>0.12486778095928799</v>
       </c>
       <c r="N23">
-        <v>3.7511310769012221E-2</v>
+        <v>3.7511310769012207E-2</v>
       </c>
       <c r="O23">
         <v>1.027785838233213E-2</v>
@@ -3740,10 +3740,10 @@
         <v>-1</v>
       </c>
       <c r="M24">
-        <v>0.13581675675881641</v>
+        <v>0.13581675675881699</v>
       </c>
       <c r="N24">
-        <v>3.6301044480938738E-2</v>
+        <v>3.6301044480938717E-2</v>
       </c>
       <c r="O24">
         <v>1.4307567892514091E-2</v>
@@ -3805,15 +3805,15 @@
       </c>
       <c r="AD24">
         <f t="shared" si="15"/>
-        <v>0.75517939599061956</v>
+        <v>0.75517939599061945</v>
       </c>
       <c r="AE24">
         <f t="shared" si="16"/>
-        <v>1.4832034996222112</v>
+        <v>1.4832034996222108</v>
       </c>
       <c r="AF24">
         <f t="shared" si="17"/>
-        <v>1.3733365737242695</v>
+        <v>1.3733365737242691</v>
       </c>
       <c r="AG24">
         <f t="shared" si="18"/>
@@ -3857,10 +3857,10 @@
         <v>-1</v>
       </c>
       <c r="M25">
-        <v>0.13376746786766491</v>
+        <v>0.13376746786766561</v>
       </c>
       <c r="N25">
-        <v>3.3505958218792133E-2</v>
+        <v>3.3505958218792098E-2</v>
       </c>
       <c r="O25">
         <v>1.345813946291196E-2</v>
@@ -3922,11 +3922,11 @@
       </c>
       <c r="AD25">
         <f t="shared" si="15"/>
-        <v>0.72802410363159176</v>
+        <v>0.72802410363159142</v>
       </c>
       <c r="AE25">
         <f t="shared" si="16"/>
-        <v>1.5175863908199041</v>
+        <v>1.5175863908199039</v>
       </c>
       <c r="AF25">
         <f t="shared" si="17"/>
@@ -3974,13 +3974,13 @@
         <v>-1</v>
       </c>
       <c r="M26">
-        <v>0.14803115562654459</v>
+        <v>0.14803115562654559</v>
       </c>
       <c r="N26">
-        <v>3.7835916974008912E-2</v>
+        <v>3.7835916974008947E-2</v>
       </c>
       <c r="O26">
-        <v>1.7552491998599679E-2</v>
+        <v>1.7552491998599672E-2</v>
       </c>
       <c r="P26">
         <v>0.99639999999999995</v>
@@ -4039,15 +4039,15 @@
       </c>
       <c r="AD26">
         <f t="shared" si="15"/>
-        <v>0.78956228718831223</v>
+        <v>0.78956228718831245</v>
       </c>
       <c r="AE26">
         <f t="shared" si="16"/>
-        <v>1.5370537639602719</v>
+        <v>1.5370537639602724</v>
       </c>
       <c r="AF26">
         <f t="shared" si="17"/>
-        <v>1.3250463482416139</v>
+        <v>1.3250463482416142</v>
       </c>
       <c r="AG26">
         <f t="shared" si="18"/>
@@ -4091,13 +4091,13 @@
         <v>-1</v>
       </c>
       <c r="M27">
-        <v>0.13507075431348611</v>
+        <v>0.13507075431348681</v>
       </c>
       <c r="N27">
-        <v>4.0824127111684323E-2</v>
+        <v>4.0824127111684337E-2</v>
       </c>
       <c r="O27">
-        <v>9.645130308286504E-3</v>
+        <v>9.6451303082865127E-3</v>
       </c>
       <c r="P27">
         <v>0.99639999999999995</v>
@@ -4156,15 +4156,15 @@
       </c>
       <c r="AD27">
         <f t="shared" si="15"/>
-        <v>0.74749147677195971</v>
+        <v>0.74749147677195993</v>
       </c>
       <c r="AE27">
         <f t="shared" si="16"/>
-        <v>1.4140282559983293</v>
+        <v>1.4140282559983297</v>
       </c>
       <c r="AF27">
         <f t="shared" si="17"/>
-        <v>1.2625252285699367</v>
+        <v>1.2625252285699371</v>
       </c>
       <c r="AG27">
         <f t="shared" si="18"/>
@@ -4208,10 +4208,10 @@
         <v>-1</v>
       </c>
       <c r="M28">
-        <v>0.11339605622286469</v>
+        <v>0.1133960562228653</v>
       </c>
       <c r="N28">
-        <v>2.928925657338504E-2</v>
+        <v>2.9289256573385051E-2</v>
       </c>
       <c r="O28">
         <v>1.007678582531339E-2</v>
@@ -4273,7 +4273,7 @@
       </c>
       <c r="AD28">
         <f t="shared" si="15"/>
-        <v>0.66653677922636956</v>
+        <v>0.66653677922636967</v>
       </c>
       <c r="AE28">
         <f t="shared" si="16"/>
@@ -4325,7 +4325,7 @@
         <v>-1</v>
       </c>
       <c r="M29">
-        <v>0.13635991884567761</v>
+        <v>0.13635991884567841</v>
       </c>
       <c r="N29">
         <v>3.6709582025640237E-2</v>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="AE29">
         <f t="shared" si="16"/>
-        <v>1.4510809155792699</v>
+        <v>1.4510809155792697</v>
       </c>
       <c r="AF29">
         <f t="shared" si="17"/>
@@ -4442,13 +4442,13 @@
         <v>-1</v>
       </c>
       <c r="M30">
-        <v>0.1224521338452579</v>
+        <v>0.1224521338452588</v>
       </c>
       <c r="N30">
-        <v>3.4066823304280819E-2</v>
+        <v>3.4066823304280798E-2</v>
       </c>
       <c r="O30">
-        <v>9.8639827603688932E-3</v>
+        <v>9.8639827603688966E-3</v>
       </c>
       <c r="P30">
         <v>0.99639999999999995</v>
@@ -4507,15 +4507,15 @@
       </c>
       <c r="AD30">
         <f t="shared" si="15"/>
-        <v>0.7015859864271714</v>
+        <v>0.70158598642717118</v>
       </c>
       <c r="AE30">
         <f t="shared" si="16"/>
-        <v>1.3971963372063452</v>
+        <v>1.397196337206345</v>
       </c>
       <c r="AF30">
         <f t="shared" si="17"/>
-        <v>1.2474967296485224</v>
+        <v>1.2474967296485222</v>
       </c>
       <c r="AG30">
         <f t="shared" si="18"/>
@@ -4559,13 +4559,13 @@
         <v>-1</v>
       </c>
       <c r="M31">
-        <v>0.1135353634263923</v>
+        <v>0.113535363426393</v>
       </c>
       <c r="N31">
-        <v>3.5362473245427427E-2</v>
+        <v>3.5362473245427413E-2</v>
       </c>
       <c r="O31">
-        <v>8.2613186007344484E-3</v>
+        <v>8.2613186007344398E-3</v>
       </c>
       <c r="P31">
         <v>0.99639999999999995</v>
@@ -4624,15 +4624,15 @@
       </c>
       <c r="AD31">
         <f t="shared" si="15"/>
-        <v>0.69561035077917388</v>
+        <v>0.69561035077917377</v>
       </c>
       <c r="AE31">
         <f t="shared" si="16"/>
-        <v>1.4148995855216477</v>
+        <v>1.4148995855216475</v>
       </c>
       <c r="AF31">
         <f t="shared" si="17"/>
-        <v>1.3100922088163405</v>
+        <v>1.3100922088163403</v>
       </c>
       <c r="AG31">
         <f t="shared" si="18"/>
@@ -4676,13 +4676,13 @@
         <v>-1</v>
       </c>
       <c r="M32">
-        <v>0.12156864847810279</v>
+        <v>0.1215686484781036</v>
       </c>
       <c r="N32">
         <v>3.1737877943178582E-2</v>
       </c>
       <c r="O32">
-        <v>1.406684567975147E-2</v>
+        <v>1.4066845679751449E-2</v>
       </c>
       <c r="P32">
         <v>0.99639999999999995</v>
@@ -4741,15 +4741,15 @@
       </c>
       <c r="AD32">
         <f t="shared" si="15"/>
-        <v>0.71928923474247397</v>
+        <v>0.71928923474247375</v>
       </c>
       <c r="AE32">
         <f t="shared" si="16"/>
-        <v>1.5104626757083812</v>
+        <v>1.5104626757083808</v>
       </c>
       <c r="AF32">
         <f t="shared" si="17"/>
-        <v>1.3731478870076192</v>
+        <v>1.3731478870076188</v>
       </c>
       <c r="AG32">
         <f t="shared" si="18"/>
@@ -4793,10 +4793,10 @@
         <v>-1</v>
       </c>
       <c r="M33">
-        <v>0.140276489116551</v>
+        <v>0.14027648911655191</v>
       </c>
       <c r="N33">
-        <v>4.3243138287783561E-2</v>
+        <v>4.3243138287783547E-2</v>
       </c>
       <c r="O33">
         <v>1.2817026076946779E-2</v>
@@ -4858,7 +4858,7 @@
       </c>
       <c r="AD33">
         <f t="shared" si="15"/>
-        <v>0.79117344096590714</v>
+        <v>0.79117344096590703</v>
       </c>
       <c r="AE33">
         <f t="shared" si="16"/>
@@ -4910,7 +4910,7 @@
         <v>-1</v>
       </c>
       <c r="M34">
-        <v>0.13904810458854269</v>
+        <v>0.13904810458854391</v>
       </c>
       <c r="N34">
         <v>3.2212933089758429E-2</v>
@@ -5027,13 +5027,13 @@
         <v>-1</v>
       </c>
       <c r="M35">
-        <v>0.1367107254432838</v>
+        <v>0.13671072544328469</v>
       </c>
       <c r="N35">
-        <v>4.3142535479400418E-2</v>
+        <v>4.3142535479400432E-2</v>
       </c>
       <c r="O35">
-        <v>1.2170112836046651E-2</v>
+        <v>1.217011283604664E-2</v>
       </c>
       <c r="P35">
         <v>0.99639999999999995</v>
@@ -5096,11 +5096,11 @@
       </c>
       <c r="AE35">
         <f t="shared" si="16"/>
-        <v>1.4876929300428148</v>
+        <v>1.487692930042815</v>
       </c>
       <c r="AF35">
         <f t="shared" si="17"/>
-        <v>1.304993798283171</v>
+        <v>1.3049937982831712</v>
       </c>
       <c r="AG35">
         <f t="shared" si="18"/>
@@ -5144,10 +5144,10 @@
         <v>-1</v>
       </c>
       <c r="M36">
-        <v>0.13226291338012999</v>
+        <v>0.13226291338013119</v>
       </c>
       <c r="N36">
-        <v>2.9891195366104299E-2</v>
+        <v>2.9891195366104309E-2</v>
       </c>
       <c r="O36">
         <v>1.3769993512398319E-2</v>
@@ -5209,7 +5209,7 @@
       </c>
       <c r="AD36">
         <f t="shared" si="15"/>
-        <v>0.70248386202809721</v>
+        <v>0.70248386202809732</v>
       </c>
       <c r="AE36">
         <f t="shared" si="16"/>
@@ -5261,10 +5261,10 @@
         <v>-1</v>
       </c>
       <c r="M37">
-        <v>0.11851240002708149</v>
+        <v>0.1185124000270824</v>
       </c>
       <c r="N37">
-        <v>3.3130678197571081E-2</v>
+        <v>3.3130678197571088E-2</v>
       </c>
       <c r="O37">
         <v>1.2143901482491309E-2</v>
@@ -5378,10 +5378,10 @@
         <v>-1</v>
       </c>
       <c r="M38">
-        <v>0.15867036847358679</v>
+        <v>0.15867036847358831</v>
       </c>
       <c r="N38">
-        <v>3.9825669155021337E-2</v>
+        <v>3.9825669155021323E-2</v>
       </c>
       <c r="O38">
         <v>1.986001787706438E-2</v>
@@ -5447,11 +5447,11 @@
       </c>
       <c r="AE38">
         <f t="shared" si="16"/>
-        <v>1.3988009479778036</v>
+        <v>1.3988009479778039</v>
       </c>
       <c r="AF38">
         <f t="shared" si="17"/>
-        <v>1.4273479060997996</v>
+        <v>1.4273479060997998</v>
       </c>
       <c r="AG38">
         <f t="shared" si="18"/>
@@ -5495,10 +5495,10 @@
         <v>-1</v>
       </c>
       <c r="M39">
-        <v>7.7492909249088887E-2</v>
+        <v>7.7492909249089401E-2</v>
       </c>
       <c r="N39">
-        <v>1.661697653430181E-2</v>
+        <v>1.661697653430182E-2</v>
       </c>
       <c r="O39">
         <v>1.372517243868834E-2</v>
@@ -5560,15 +5560,15 @@
       </c>
       <c r="AD39">
         <f t="shared" si="15"/>
-        <v>0.5801075233233024</v>
+        <v>0.58010752332330251</v>
       </c>
       <c r="AE39">
         <f t="shared" si="16"/>
-        <v>1.0461621686896139</v>
+        <v>1.0461621686896143</v>
       </c>
       <c r="AF39">
         <f t="shared" si="17"/>
-        <v>0.90186393852552926</v>
+        <v>0.9018639385255296</v>
       </c>
       <c r="AG39">
         <f t="shared" si="18"/>
@@ -5612,13 +5612,13 @@
         <v>-1</v>
       </c>
       <c r="M40">
-        <v>0.1004860018703238</v>
+        <v>0.1004860018703211</v>
       </c>
       <c r="N40">
-        <v>1.378634247936009E-2</v>
+        <v>1.378634247936013E-2</v>
       </c>
       <c r="O40">
-        <v>5.2821992154628962E-3</v>
+        <v>5.2821992154628841E-3</v>
       </c>
       <c r="P40">
         <v>0.99639999999999995</v>
@@ -5677,15 +5677,15 @@
       </c>
       <c r="AD40">
         <f t="shared" si="15"/>
-        <v>0.46605464536631147</v>
+        <v>0.4660546453663118</v>
       </c>
       <c r="AE40">
         <f t="shared" si="16"/>
-        <v>1.11498003009928</v>
+        <v>1.1149800300992805</v>
       </c>
       <c r="AF40">
         <f t="shared" si="17"/>
-        <v>0.68825927783906171</v>
+        <v>0.68825927783906193</v>
       </c>
       <c r="AG40">
         <f t="shared" si="18"/>
@@ -5729,13 +5729,13 @@
         <v>-1</v>
       </c>
       <c r="M41">
-        <v>2.251836339486649E-2</v>
+        <v>2.2518363394864141E-2</v>
       </c>
       <c r="N41">
-        <v>3.5359732526322157E-2</v>
+        <v>3.5359732526322171E-2</v>
       </c>
       <c r="O41">
-        <v>4.31743336602434E-3</v>
+        <v>4.3174333660243496E-3</v>
       </c>
       <c r="P41">
         <v>0.99639999999999995</v>
@@ -5794,15 +5794,15 @@
       </c>
       <c r="AD41">
         <f t="shared" si="15"/>
-        <v>0.64892538473296857</v>
+        <v>0.64892538473296879</v>
       </c>
       <c r="AE41">
         <f t="shared" si="16"/>
-        <v>1.4246268984688109</v>
+        <v>1.4246268984688111</v>
       </c>
       <c r="AF41">
         <f t="shared" si="17"/>
-        <v>0.97577184826630881</v>
+        <v>0.97577184826630903</v>
       </c>
       <c r="AG41">
         <f t="shared" si="18"/>
@@ -5846,13 +5846,13 @@
         <v>-1</v>
       </c>
       <c r="M42">
-        <v>8.2659944117324122E-2</v>
+        <v>8.2659944117325121E-2</v>
       </c>
       <c r="N42">
         <v>3.4847092556515212E-2</v>
       </c>
       <c r="O42">
-        <v>1.8690036361776581E-2</v>
+        <v>1.8690036361776571E-2</v>
       </c>
       <c r="P42">
         <v>0.99639999999999995</v>
@@ -5963,13 +5963,13 @@
         <v>-1</v>
       </c>
       <c r="M43">
-        <v>9.160771211071965E-2</v>
+        <v>9.1607712110720482E-2</v>
       </c>
       <c r="N43">
-        <v>3.3365292703850247E-2</v>
+        <v>3.3365292703850261E-2</v>
       </c>
       <c r="O43">
-        <v>6.3553570494151784E-3</v>
+        <v>6.3553570494151732E-3</v>
       </c>
       <c r="P43">
         <v>0.99639999999999995</v>
@@ -6080,7 +6080,7 @@
         <v>-1</v>
       </c>
       <c r="M44">
-        <v>9.1330534612419412E-2</v>
+        <v>9.1330534612420175E-2</v>
       </c>
       <c r="N44">
         <v>3.3633664135465917E-2</v>
@@ -6149,11 +6149,11 @@
       </c>
       <c r="AE44">
         <f t="shared" si="16"/>
-        <v>1.4850258917933312</v>
+        <v>1.4850258917933314</v>
       </c>
       <c r="AF44">
         <f t="shared" si="17"/>
-        <v>1.3259159748154741</v>
+        <v>1.3259159748154743</v>
       </c>
       <c r="AG44">
         <f t="shared" si="18"/>
@@ -6197,13 +6197,13 @@
         <v>-1</v>
       </c>
       <c r="M45">
-        <v>0.1409975545711451</v>
+        <v>0.14099755457114671</v>
       </c>
       <c r="N45">
-        <v>3.9363045837057513E-2</v>
+        <v>3.9363045837057548E-2</v>
       </c>
       <c r="O45">
-        <v>1.6130217368263599E-2</v>
+        <v>1.6130217368263582E-2</v>
       </c>
       <c r="P45">
         <v>0.99639999999999995</v>
@@ -6262,7 +6262,7 @@
       </c>
       <c r="AD45">
         <f t="shared" si="15"/>
-        <v>0.79024745568830679</v>
+        <v>0.7902474556883069</v>
       </c>
       <c r="AE45">
         <f t="shared" si="16"/>
@@ -6314,10 +6314,10 @@
         <v>-1</v>
       </c>
       <c r="M46">
-        <v>0.1322436429314793</v>
+        <v>0.1322436429314803</v>
       </c>
       <c r="N46">
-        <v>3.3342027404730259E-2</v>
+        <v>3.3342027404730239E-2</v>
       </c>
       <c r="O46">
         <v>1.0395340938243141E-2</v>
@@ -6379,7 +6379,7 @@
       </c>
       <c r="AD46">
         <f t="shared" si="15"/>
-        <v>0.70101310835204722</v>
+        <v>0.70101310835204711</v>
       </c>
       <c r="AE46">
         <f t="shared" si="16"/>
@@ -6431,10 +6431,10 @@
         <v>-1</v>
       </c>
       <c r="M47">
-        <v>0.14225503659926991</v>
+        <v>0.14225503659927119</v>
       </c>
       <c r="N47">
-        <v>3.03620237060927E-2</v>
+        <v>3.036202370609271E-2</v>
       </c>
       <c r="O47">
         <v>1.3509725237132749E-2</v>
@@ -6496,15 +6496,15 @@
       </c>
       <c r="AD47">
         <f t="shared" si="15"/>
-        <v>0.70418802039749406</v>
+        <v>0.70418802039749417</v>
       </c>
       <c r="AE47">
         <f t="shared" si="16"/>
-        <v>1.4980488730746333</v>
+        <v>1.4980488730746335</v>
       </c>
       <c r="AF47">
         <f t="shared" si="17"/>
-        <v>1.3375436366737796</v>
+        <v>1.3375436366737798</v>
       </c>
       <c r="AG47">
         <f t="shared" si="18"/>
@@ -6548,7 +6548,7 @@
         <v>-1</v>
       </c>
       <c r="M48">
-        <v>0.14494529735019629</v>
+        <v>0.14494529735019751</v>
       </c>
       <c r="N48">
         <v>4.2767273757541427E-2</v>
@@ -6617,11 +6617,11 @@
       </c>
       <c r="AE48">
         <f t="shared" si="16"/>
-        <v>1.5479734997136194</v>
+        <v>1.5479734997136196</v>
       </c>
       <c r="AF48">
         <f t="shared" si="17"/>
-        <v>1.3578714909768592</v>
+        <v>1.3578714909768594</v>
       </c>
       <c r="AG48">
         <f t="shared" si="18"/>
@@ -6665,13 +6665,13 @@
         <v>-1</v>
       </c>
       <c r="M49">
-        <v>0.12701526731514409</v>
+        <v>0.1270152673151454</v>
       </c>
       <c r="N49">
-        <v>3.5778357957153263E-2</v>
+        <v>3.5778357957153312E-2</v>
       </c>
       <c r="O49">
-        <v>1.4665300805489371E-2</v>
+        <v>1.4665300805489339E-2</v>
       </c>
       <c r="P49">
         <v>0.99639999999999995</v>
@@ -6730,7 +6730,7 @@
       </c>
       <c r="AD49">
         <f t="shared" si="15"/>
-        <v>0.75411264703648007</v>
+        <v>0.75411264703648029</v>
       </c>
       <c r="AE49">
         <f t="shared" si="16"/>
@@ -6782,10 +6782,10 @@
         <v>-1</v>
       </c>
       <c r="M50">
-        <v>0.1295621379460723</v>
+        <v>0.12956213794607341</v>
       </c>
       <c r="N50">
-        <v>3.779063969131629E-2</v>
+        <v>3.7790639691316269E-2</v>
       </c>
       <c r="O50">
         <v>7.7108319671635849E-3</v>
@@ -6847,15 +6847,15 @@
       </c>
       <c r="AD50">
         <f t="shared" si="15"/>
-        <v>0.70734857051624733</v>
+        <v>0.70734857051624711</v>
       </c>
       <c r="AE50">
         <f t="shared" si="16"/>
-        <v>1.4245643108208803</v>
+        <v>1.4245643108208799</v>
       </c>
       <c r="AF50">
         <f t="shared" si="17"/>
-        <v>1.319041028537852</v>
+        <v>1.3190410285378515</v>
       </c>
       <c r="AG50">
         <f t="shared" si="18"/>
@@ -6896,10 +6896,10 @@
         <v>-1</v>
       </c>
       <c r="M51">
-        <v>0.1269463238118059</v>
+        <v>0.12694632381180729</v>
       </c>
       <c r="N51">
-        <v>3.4394137414869783E-2</v>
+        <v>3.4394137414869769E-2</v>
       </c>
       <c r="O51">
         <v>1.134121199851369E-2</v>
@@ -6961,15 +6961,15 @@
       </c>
       <c r="AD51">
         <f t="shared" si="15"/>
-        <v>0.71721574030463298</v>
+        <v>0.71721574030463286</v>
       </c>
       <c r="AE51" s="1">
         <f t="shared" si="16"/>
-        <v>0.71721574030463298</v>
+        <v>0.71721574030463286</v>
       </c>
       <c r="AF51" s="1">
         <f t="shared" si="17"/>
-        <v>-2.5343312378255583E-2</v>
+        <v>-2.5343312378255576E-2</v>
       </c>
       <c r="AG51">
         <f t="shared" si="18"/>
@@ -7055,11 +7055,11 @@
       </c>
       <c r="AE52" s="1">
         <f t="shared" si="16"/>
-        <v>0.49387085412603582</v>
+        <v>0.49387085412603665</v>
       </c>
       <c r="AF52" s="1">
         <f t="shared" si="17"/>
-        <v>-1.7124509505063654E-2</v>
+        <v>-1.7124509505063685E-2</v>
       </c>
       <c r="AG52" s="1">
         <f t="shared" si="18"/>
@@ -7103,13 +7103,13 @@
         <v>-1</v>
       </c>
       <c r="M53">
-        <v>6.2018275607622193E-2</v>
+        <v>6.2018275607623338E-2</v>
       </c>
       <c r="N53">
-        <v>7.7358468391496979E-3</v>
+        <v>7.7358468391497603E-3</v>
       </c>
       <c r="O53">
-        <v>1.7612269362436549E-2</v>
+        <v>1.7612269362436529E-2</v>
       </c>
       <c r="P53">
         <v>0.99639999999999995</v>
@@ -7168,15 +7168,15 @@
       </c>
       <c r="AD53">
         <f t="shared" si="15"/>
-        <v>0.49387085412603582</v>
+        <v>0.49387085412603665</v>
       </c>
       <c r="AE53">
         <f t="shared" si="16"/>
-        <v>1.024389017905142</v>
+        <v>1.0243890179051434</v>
       </c>
       <c r="AF53">
         <f t="shared" si="17"/>
-        <v>0.80030392023839214</v>
+        <v>0.80030392023839325</v>
       </c>
       <c r="AG53">
         <f t="shared" si="18"/>
@@ -7220,13 +7220,13 @@
         <v>-1</v>
       </c>
       <c r="M54">
-        <v>6.4645126663146021E-2</v>
+        <v>6.4645126663145203E-2</v>
       </c>
       <c r="N54">
-        <v>1.946841593623173E-2</v>
+        <v>1.9468415936231762E-2</v>
       </c>
       <c r="O54">
-        <v>5.504521584815506E-3</v>
+        <v>5.5045215848155138E-3</v>
       </c>
       <c r="P54">
         <v>0.99639999999999995</v>
@@ -7285,15 +7285,15 @@
       </c>
       <c r="AD54">
         <f t="shared" si="15"/>
-        <v>0.53051816377910621</v>
+        <v>0.53051816377910666</v>
       </c>
       <c r="AE54">
         <f t="shared" si="16"/>
-        <v>1.2289933791678007</v>
+        <v>1.2289933791678012</v>
       </c>
       <c r="AF54">
         <f t="shared" si="17"/>
-        <v>0.99112369287725866</v>
+        <v>0.99112369287725899</v>
       </c>
       <c r="AG54">
         <f t="shared" si="18"/>
@@ -7337,13 +7337,13 @@
         <v>-1</v>
       </c>
       <c r="M55">
-        <v>0.10749251549728089</v>
+        <v>0.1074925154972802</v>
       </c>
       <c r="N55">
-        <v>3.3486682158044297E-2</v>
+        <v>3.3486682158044269E-2</v>
       </c>
       <c r="O55">
-        <v>9.9972929879252864E-3</v>
+        <v>9.9972929879252916E-3</v>
       </c>
       <c r="P55">
         <v>0.99639999999999995</v>
@@ -7406,11 +7406,11 @@
       </c>
       <c r="AE55">
         <f t="shared" si="16"/>
-        <v>1.4377040603895508</v>
+        <v>1.4377040603895506</v>
       </c>
       <c r="AF55">
         <f t="shared" si="17"/>
-        <v>1.2611439126224131</v>
+        <v>1.2611439126224129</v>
       </c>
       <c r="AG55">
         <f t="shared" si="18"/>
@@ -7454,10 +7454,10 @@
         <v>-1</v>
       </c>
       <c r="M56">
-        <v>0.1348916034416712</v>
+        <v>0.13489160344167059</v>
       </c>
       <c r="N56">
-        <v>3.6859597616478931E-2</v>
+        <v>3.6859597616478897E-2</v>
       </c>
       <c r="O56">
         <v>1.181833878643168E-2</v>
@@ -7519,7 +7519,7 @@
       </c>
       <c r="AD56">
         <f t="shared" si="15"/>
-        <v>0.73922884500085639</v>
+        <v>0.73922884500085617</v>
       </c>
       <c r="AE56">
         <f t="shared" si="16"/>
@@ -7571,13 +7571,13 @@
         <v>-1</v>
       </c>
       <c r="M57">
-        <v>0.1550701713552671</v>
+        <v>0.15507017135526621</v>
       </c>
       <c r="N57">
-        <v>3.8720908955532547E-2</v>
+        <v>3.8720908955532589E-2</v>
       </c>
       <c r="O57">
-        <v>1.9908944450465631E-2</v>
+        <v>1.9908944450465621E-2</v>
       </c>
       <c r="P57">
         <v>0.99639999999999995</v>
@@ -7636,15 +7636,15 @@
       </c>
       <c r="AD57">
         <f t="shared" si="15"/>
-        <v>0.81137196568887426</v>
+        <v>0.81137196568887449</v>
       </c>
       <c r="AE57">
         <f t="shared" si="16"/>
-        <v>1.5525556903731947</v>
+        <v>1.552555690373195</v>
       </c>
       <c r="AF57">
         <f t="shared" si="17"/>
-        <v>1.3862104378332094</v>
+        <v>1.3862104378332096</v>
       </c>
       <c r="AG57">
         <f t="shared" si="18"/>
@@ -7688,13 +7688,13 @@
         <v>-1</v>
       </c>
       <c r="M58">
-        <v>0.13905297938532279</v>
+        <v>0.13905297938532221</v>
       </c>
       <c r="N58">
         <v>3.4912089222745857E-2</v>
       </c>
       <c r="O58">
-        <v>1.380353261305072E-2</v>
+        <v>1.380353261305073E-2</v>
       </c>
       <c r="P58">
         <v>0.99639999999999995</v>
@@ -7757,11 +7757,11 @@
       </c>
       <c r="AE58">
         <f t="shared" si="16"/>
-        <v>1.5456877290735607</v>
+        <v>1.5456877290735609</v>
       </c>
       <c r="AF58">
         <f t="shared" si="17"/>
-        <v>1.3800783295299648</v>
+        <v>1.380078329529965</v>
       </c>
       <c r="AG58">
         <f t="shared" si="18"/>
@@ -7805,13 +7805,13 @@
         <v>-1</v>
       </c>
       <c r="M59">
-        <v>0.1469018589256669</v>
+        <v>0.1469018589256661</v>
       </c>
       <c r="N59">
-        <v>3.5559132018004792E-2</v>
+        <v>3.5559132018004827E-2</v>
       </c>
       <c r="O59">
-        <v>2.2431039310977931E-2</v>
+        <v>2.243103931097792E-2</v>
       </c>
       <c r="P59">
         <v>0.99639999999999995</v>
@@ -7870,15 +7870,15 @@
       </c>
       <c r="AD59">
         <f t="shared" si="15"/>
-        <v>0.80450400438924019</v>
+        <v>0.80450400438924041</v>
       </c>
       <c r="AE59">
         <f t="shared" si="16"/>
-        <v>1.5877080565491317</v>
+        <v>1.5877080565491319</v>
       </c>
       <c r="AF59">
         <f t="shared" si="17"/>
-        <v>1.4175964790617246</v>
+        <v>1.4175964790617248</v>
       </c>
       <c r="AG59">
         <f t="shared" si="18"/>
@@ -7922,10 +7922,10 @@
         <v>-1</v>
       </c>
       <c r="M60">
-        <v>0.1428924859169427</v>
+        <v>0.14289248591694209</v>
       </c>
       <c r="N60">
-        <v>3.7973679740547613E-2</v>
+        <v>3.7973679740547599E-2</v>
       </c>
       <c r="O60">
         <v>1.650052014218931E-2</v>
@@ -8039,13 +8039,13 @@
         <v>-1</v>
       </c>
       <c r="M61">
-        <v>0.15648920761121729</v>
+        <v>0.15648920761121671</v>
       </c>
       <c r="N61">
-        <v>4.0220660829513193E-2</v>
+        <v>4.0220660829513158E-2</v>
       </c>
       <c r="O61">
-        <v>2.0729015268606061E-2</v>
+        <v>2.0729015268606078E-2</v>
       </c>
       <c r="P61">
         <v>0.99639999999999995</v>
@@ -8104,7 +8104,7 @@
       </c>
       <c r="AD61">
         <f t="shared" si="15"/>
-        <v>0.82690799565511475</v>
+        <v>0.82690799565511464</v>
       </c>
       <c r="AE61">
         <f t="shared" si="16"/>
@@ -8156,13 +8156,13 @@
         <v>-1</v>
       </c>
       <c r="M62">
-        <v>0.114190055369795</v>
+        <v>0.11419005536979469</v>
       </c>
       <c r="N62">
-        <v>4.1054617350940417E-2</v>
+        <v>4.1054617350940431E-2</v>
       </c>
       <c r="O62">
-        <v>7.1910946895962311E-3</v>
+        <v>7.1910946895962337E-3</v>
       </c>
       <c r="P62">
         <v>0.99639999999999995</v>
@@ -8221,7 +8221,7 @@
       </c>
       <c r="AD62">
         <f t="shared" si="15"/>
-        <v>0.72429865676779215</v>
+        <v>0.72429865676779226</v>
       </c>
       <c r="AE62">
         <f t="shared" si="16"/>
@@ -8264,7 +8264,7 @@
       </c>
       <c r="I63">
         <f t="shared" si="1"/>
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="K63">
         <v>2</v>
@@ -8273,13 +8273,13 @@
         <v>-1</v>
       </c>
       <c r="M63">
-        <v>0.13026011149808131</v>
+        <v>0.13026011149808089</v>
       </c>
       <c r="N63">
         <v>3.0609221583568689E-2</v>
       </c>
       <c r="O63">
-        <v>1.288252195207854E-2</v>
+        <v>1.288252195207853E-2</v>
       </c>
       <c r="P63">
         <v>0.99639999999999995</v>
@@ -8290,7 +8290,7 @@
       </c>
       <c r="R63">
         <f t="shared" si="3"/>
-        <v>1.08</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="S63">
         <f t="shared" si="4"/>
@@ -8298,7 +8298,7 @@
       </c>
       <c r="T63">
         <f t="shared" si="5"/>
-        <v>0.36</v>
+        <v>0.38</v>
       </c>
       <c r="U63">
         <f t="shared" si="6"/>
@@ -8338,15 +8338,15 @@
       </c>
       <c r="AD63">
         <f t="shared" si="15"/>
-        <v>0.70114364733629031</v>
+        <v>0.7011436473362902</v>
       </c>
       <c r="AE63">
         <f t="shared" si="16"/>
-        <v>1.4302740565690151</v>
+        <v>1.4380343329395786</v>
       </c>
       <c r="AF63">
         <f t="shared" si="17"/>
-        <v>1.3243278301564954</v>
+        <v>1.3073039390359804</v>
       </c>
       <c r="AG63">
         <f t="shared" si="18"/>
@@ -8377,7 +8377,7 @@
       </c>
       <c r="H64">
         <f t="shared" si="0"/>
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="I64">
         <f t="shared" si="1"/>
@@ -8390,20 +8390,20 @@
         <v>-1</v>
       </c>
       <c r="M64">
-        <v>0.1199663509496231</v>
+        <v>0.1199663509496228</v>
       </c>
       <c r="N64">
-        <v>3.3296449768215913E-2</v>
+        <v>3.5087704132897718E-2</v>
       </c>
       <c r="O64">
-        <v>1.3800753514793729E-2</v>
+        <v>1.309574716113616E-2</v>
       </c>
       <c r="P64">
         <v>0.99639999999999995</v>
       </c>
       <c r="Q64">
         <f t="shared" si="2"/>
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="R64">
         <f t="shared" si="3"/>
@@ -8423,15 +8423,15 @@
       </c>
       <c r="V64">
         <f t="shared" si="7"/>
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="W64">
         <f t="shared" si="8"/>
-        <v>0.36</v>
+        <v>0.33999999999999997</v>
       </c>
       <c r="X64">
         <f t="shared" si="9"/>
-        <v>0.36</v>
+        <v>0.38</v>
       </c>
       <c r="Y64" s="2">
         <f t="shared" si="19"/>
@@ -8455,19 +8455,19 @@
       </c>
       <c r="AD64">
         <f t="shared" si="15"/>
-        <v>0.72913040923272487</v>
+        <v>0.7368906856032883</v>
       </c>
       <c r="AE64">
         <f t="shared" si="16"/>
-        <v>1.5424913118030759</v>
+        <v>1.5102217982765742</v>
       </c>
       <c r="AF64">
         <f t="shared" si="17"/>
-        <v>1.3530625542132246</v>
+        <v>1.3247559634005037</v>
       </c>
       <c r="AG64">
         <f t="shared" si="18"/>
-        <v>111.1111111111111</v>
+        <v>107.14285714285714</v>
       </c>
     </row>
     <row r="65" spans="1:33" x14ac:dyDescent="0.2">
@@ -8484,7 +8484,7 @@
         <v>28</v>
       </c>
       <c r="E65">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F65">
         <v>378</v>
@@ -8507,28 +8507,28 @@
         <v>-1</v>
       </c>
       <c r="M65">
-        <v>0.14929247373138091</v>
+        <v>0.13857684217778191</v>
       </c>
       <c r="N65">
-        <v>3.8941840055516701E-2</v>
+        <v>3.7310119065896923E-2</v>
       </c>
       <c r="O65">
-        <v>1.997968350715389E-2</v>
+        <v>1.5777318277010909E-2</v>
       </c>
       <c r="P65">
         <v>0.99639999999999995</v>
       </c>
       <c r="Q65">
         <f t="shared" si="2"/>
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="R65">
         <f t="shared" si="3"/>
-        <v>1.1399999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="S65">
         <f t="shared" si="4"/>
-        <v>0.76</v>
+        <v>0.74</v>
       </c>
       <c r="T65">
         <f t="shared" si="5"/>
@@ -8536,7 +8536,7 @@
       </c>
       <c r="U65">
         <f t="shared" si="6"/>
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="V65">
         <f t="shared" si="7"/>
@@ -8544,7 +8544,7 @@
       </c>
       <c r="W65">
         <f t="shared" si="8"/>
-        <v>0.33999999999999997</v>
+        <v>0.32</v>
       </c>
       <c r="X65">
         <f t="shared" si="9"/>
@@ -8572,19 +8572,19 @@
       </c>
       <c r="AD65">
         <f t="shared" si="15"/>
-        <v>0.8133609025703511</v>
+        <v>0.77333111267328591</v>
       </c>
       <c r="AE65">
         <f t="shared" si="16"/>
-        <v>1.5114125577307718</v>
+        <v>1.4713827678337064</v>
       </c>
       <c r="AF65">
         <f t="shared" si="17"/>
-        <v>1.3258004892375193</v>
+        <v>1.3137346141372377</v>
       </c>
       <c r="AG65">
         <f t="shared" si="18"/>
-        <v>100</v>
+        <v>103.44827586206897</v>
       </c>
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.2">
@@ -8624,13 +8624,13 @@
         <v>-1</v>
       </c>
       <c r="M66">
-        <v>0.1209932340514371</v>
+        <v>0.120993234051437</v>
       </c>
       <c r="N66">
-        <v>3.2397625390807969E-2</v>
+        <v>3.2397625390807948E-2</v>
       </c>
       <c r="O66">
-        <v>1.0867400865245911E-2</v>
+        <v>1.08674008652459E-2</v>
       </c>
       <c r="P66">
         <v>0.99639999999999995</v>
@@ -8689,11 +8689,11 @@
       </c>
       <c r="AD66">
         <f t="shared" si="15"/>
-        <v>0.69805165516042056</v>
+        <v>0.69805165516042045</v>
       </c>
       <c r="AE66">
         <f t="shared" si="16"/>
-        <v>1.5087320962673967</v>
+        <v>1.5087320962673969</v>
       </c>
       <c r="AF66">
         <f t="shared" si="17"/>
@@ -8741,13 +8741,13 @@
         <v>-1</v>
       </c>
       <c r="M67">
-        <v>0.13393018134387669</v>
+        <v>0.13393018134387649</v>
       </c>
       <c r="N67">
-        <v>4.0448079247052397E-2</v>
+        <v>4.0448079247052418E-2</v>
       </c>
       <c r="O67">
-        <v>1.7997651844659079E-2</v>
+        <v>1.7997651844659068E-2</v>
       </c>
       <c r="P67">
         <v>0.99639999999999995</v>
@@ -8806,15 +8806,15 @@
       </c>
       <c r="AD67">
         <f t="shared" ref="AD67:AD81" si="34">2 * SQRT(2 * P67 * N67 - N67 * N67) + 2 * SQRT(2 * AC67 * O67 - O67 * O67)</f>
-        <v>0.81068044110697612</v>
+        <v>0.81068044110697635</v>
       </c>
       <c r="AE67">
         <f t="shared" ref="AE67:AE80" si="35">AD67+AD68</f>
-        <v>1.5102736149919149</v>
+        <v>1.5102736149919151</v>
       </c>
       <c r="AF67">
         <f t="shared" ref="AF67:AF80" si="36">AE67/R67</f>
-        <v>1.3484585848142097</v>
+        <v>1.3484585848142099</v>
       </c>
       <c r="AG67">
         <f t="shared" ref="AG67:AG81" si="37">60/Q67</f>
@@ -8858,13 +8858,13 @@
         <v>-1</v>
       </c>
       <c r="M68">
-        <v>0.13128151199029081</v>
+        <v>0.1312815119902907</v>
       </c>
       <c r="N68">
         <v>3.1777689441312602E-2</v>
       </c>
       <c r="O68">
-        <v>1.1595318245486239E-2</v>
+        <v>1.159531824548625E-2</v>
       </c>
       <c r="P68">
         <v>0.99639999999999995</v>
@@ -8927,7 +8927,7 @@
       </c>
       <c r="AE68">
         <f t="shared" si="35"/>
-        <v>1.5333509041697913</v>
+        <v>1.533350904169791</v>
       </c>
       <c r="AF68">
         <f t="shared" si="36"/>
@@ -8975,13 +8975,13 @@
         <v>-1</v>
       </c>
       <c r="M69">
-        <v>0.14261010988455339</v>
+        <v>0.14261010988455319</v>
       </c>
       <c r="N69">
-        <v>4.4593842711454668E-2</v>
+        <v>4.459384271145464E-2</v>
       </c>
       <c r="O69">
-        <v>1.7353878460748359E-2</v>
+        <v>1.7353878460748349E-2</v>
       </c>
       <c r="P69">
         <v>0.99639999999999995</v>
@@ -9040,15 +9040,15 @@
       </c>
       <c r="AD69">
         <f t="shared" si="34"/>
-        <v>0.83375773028485245</v>
+        <v>0.83375773028485223</v>
       </c>
       <c r="AE69">
         <f t="shared" si="35"/>
-        <v>1.5454974887982438</v>
+        <v>1.5454974887982433</v>
       </c>
       <c r="AF69">
         <f t="shared" si="36"/>
-        <v>1.3323254213777964</v>
+        <v>1.332325421377796</v>
       </c>
       <c r="AG69">
         <f t="shared" si="37"/>
@@ -9092,13 +9092,13 @@
         <v>-1</v>
       </c>
       <c r="M70">
-        <v>0.12852076549027031</v>
+        <v>0.12852076549027019</v>
       </c>
       <c r="N70">
-        <v>3.5195503001050073E-2</v>
+        <v>3.5195503001050038E-2</v>
       </c>
       <c r="O70">
-        <v>1.0060970650612551E-2</v>
+        <v>1.006097065061254E-2</v>
       </c>
       <c r="P70">
         <v>0.99639999999999995</v>
@@ -9157,15 +9157,15 @@
       </c>
       <c r="AD70">
         <f t="shared" si="34"/>
-        <v>0.71173975851339133</v>
+        <v>0.71173975851339111</v>
       </c>
       <c r="AE70">
         <f t="shared" si="35"/>
-        <v>1.4184536728053638</v>
+        <v>1.4184536728053636</v>
       </c>
       <c r="AF70">
         <f t="shared" si="36"/>
-        <v>1.2664764935762176</v>
+        <v>1.2664764935762174</v>
       </c>
       <c r="AG70">
         <f t="shared" si="37"/>
@@ -9209,13 +9209,13 @@
         <v>-1</v>
       </c>
       <c r="M71">
-        <v>0.118127718152407</v>
+        <v>0.1181277181524069</v>
       </c>
       <c r="N71">
-        <v>3.2867589985157757E-2</v>
+        <v>3.286758998515775E-2</v>
       </c>
       <c r="O71">
-        <v>1.145171847843621E-2</v>
+        <v>1.1451718478436221E-2</v>
       </c>
       <c r="P71">
         <v>0.99639999999999995</v>
@@ -9274,15 +9274,15 @@
       </c>
       <c r="AD71">
         <f t="shared" si="34"/>
-        <v>0.70671391429197239</v>
+        <v>0.7067139142919725</v>
       </c>
       <c r="AE71">
         <f t="shared" si="35"/>
-        <v>1.4289488685070473</v>
+        <v>1.4289488685070471</v>
       </c>
       <c r="AF71">
         <f t="shared" si="36"/>
-        <v>1.2758472040241493</v>
+        <v>1.2758472040241491</v>
       </c>
       <c r="AG71">
         <f t="shared" si="37"/>
@@ -9329,10 +9329,10 @@
         <v>0.1358668302626915</v>
       </c>
       <c r="N72">
-        <v>3.6803997448620743E-2</v>
+        <v>3.6803997448620722E-2</v>
       </c>
       <c r="O72">
-        <v>9.9364274632791627E-3</v>
+        <v>9.9364274632791679E-3</v>
       </c>
       <c r="P72">
         <v>0.99639999999999995</v>
@@ -9391,15 +9391,15 @@
       </c>
       <c r="AD72">
         <f t="shared" si="34"/>
-        <v>0.72223495421507478</v>
+        <v>0.72223495421507455</v>
       </c>
       <c r="AE72">
         <f t="shared" si="35"/>
-        <v>1.4761703306367049</v>
+        <v>1.4761703306367044</v>
       </c>
       <c r="AF72">
         <f t="shared" si="36"/>
-        <v>1.3180092237827721</v>
+        <v>1.3180092237827716</v>
       </c>
       <c r="AG72">
         <f t="shared" si="37"/>
@@ -9446,7 +9446,7 @@
         <v>0.13562476077379271</v>
       </c>
       <c r="N73">
-        <v>3.5396965795977849E-2</v>
+        <v>3.5396965795977828E-2</v>
       </c>
       <c r="O73">
         <v>1.501236265384028E-2</v>
@@ -9508,7 +9508,7 @@
       </c>
       <c r="AD73">
         <f t="shared" si="34"/>
-        <v>0.75393537642163011</v>
+        <v>0.75393537642163</v>
       </c>
       <c r="AE73">
         <f t="shared" si="35"/>
@@ -9560,10 +9560,10 @@
         <v>-1</v>
       </c>
       <c r="M74">
-        <v>0.1244468708518592</v>
+        <v>0.12444687085185931</v>
       </c>
       <c r="N74">
-        <v>2.9397338847165791E-2</v>
+        <v>2.9397338847165781E-2</v>
       </c>
       <c r="O74">
         <v>1.454417312410719E-2</v>
@@ -9677,7 +9677,7 @@
         <v>-1</v>
       </c>
       <c r="M75">
-        <v>0.13765248521878501</v>
+        <v>0.13765248521878509</v>
       </c>
       <c r="N75">
         <v>4.0336664449592607E-2</v>
@@ -9746,11 +9746,11 @@
       </c>
       <c r="AE75">
         <f t="shared" si="35"/>
-        <v>1.533707053030358</v>
+        <v>1.5337070530303576</v>
       </c>
       <c r="AF75">
         <f t="shared" si="36"/>
-        <v>1.2997517398562357</v>
+        <v>1.2997517398562353</v>
       </c>
       <c r="AG75">
         <f t="shared" si="37"/>
@@ -9794,13 +9794,13 @@
         <v>-1</v>
       </c>
       <c r="M76">
-        <v>0.12195439530863469</v>
+        <v>0.12195439530863481</v>
       </c>
       <c r="N76">
-        <v>3.2441144268311871E-2</v>
+        <v>3.2441144268311843E-2</v>
       </c>
       <c r="O76">
-        <v>1.324996981898576E-2</v>
+        <v>1.3249969818985749E-2</v>
       </c>
       <c r="P76">
         <v>0.99639999999999995</v>
@@ -9859,15 +9859,15 @@
       </c>
       <c r="AD76">
         <f t="shared" si="34"/>
-        <v>0.71830471909130855</v>
+        <v>0.71830471909130811</v>
       </c>
       <c r="AE76">
         <f t="shared" si="35"/>
-        <v>1.4546594854945343</v>
+        <v>1.4546594854945336</v>
       </c>
       <c r="AF76">
         <f t="shared" si="36"/>
-        <v>1.2988031120486911</v>
+        <v>1.2988031120486907</v>
       </c>
       <c r="AG76">
         <f t="shared" si="37"/>
@@ -9911,13 +9911,13 @@
         <v>-1</v>
       </c>
       <c r="M77">
-        <v>0.13900619347081411</v>
+        <v>0.1390061934708143</v>
       </c>
       <c r="N77">
-        <v>3.3230259804911511E-2</v>
+        <v>3.323025980491149E-2</v>
       </c>
       <c r="O77">
-        <v>1.481210508685387E-2</v>
+        <v>1.481210508685386E-2</v>
       </c>
       <c r="P77">
         <v>0.99639999999999995</v>
@@ -9976,15 +9976,15 @@
       </c>
       <c r="AD77">
         <f t="shared" si="34"/>
-        <v>0.73635476640322572</v>
+        <v>0.7363547664032255</v>
       </c>
       <c r="AE77">
         <f t="shared" si="35"/>
-        <v>1.5353212042658679</v>
+        <v>1.5353212042658677</v>
       </c>
       <c r="AF77">
         <f t="shared" si="36"/>
-        <v>1.3235527622981622</v>
+        <v>1.323552762298162</v>
       </c>
       <c r="AG77">
         <f t="shared" si="37"/>
@@ -10028,10 +10028,10 @@
         <v>-1</v>
       </c>
       <c r="M78">
-        <v>0.13896762250391739</v>
+        <v>0.13896762250391759</v>
       </c>
       <c r="N78">
-        <v>4.3107399480909983E-2</v>
+        <v>4.3107399480909969E-2</v>
       </c>
       <c r="O78">
         <v>1.391431265963794E-2</v>
@@ -10093,7 +10093,7 @@
       </c>
       <c r="AD78">
         <f t="shared" si="34"/>
-        <v>0.79896643786264232</v>
+        <v>0.79896643786264221</v>
       </c>
       <c r="AE78">
         <f t="shared" si="35"/>
@@ -10145,13 +10145,13 @@
         <v>-1</v>
       </c>
       <c r="M79">
-        <v>0.1181093838779627</v>
+        <v>0.1181093838779629</v>
       </c>
       <c r="N79">
-        <v>3.1888642096832988E-2</v>
+        <v>3.1888642096832967E-2</v>
       </c>
       <c r="O79">
-        <v>1.025369105141026E-2</v>
+        <v>1.0253691051410271E-2</v>
       </c>
       <c r="P79">
         <v>0.99639999999999995</v>
@@ -10262,10 +10262,10 @@
         <v>-1</v>
       </c>
       <c r="M80">
-        <v>0.13349025854761831</v>
+        <v>0.13349025854761859</v>
       </c>
       <c r="N80">
-        <v>3.5761978642232878E-2</v>
+        <v>3.5761978642232857E-2</v>
       </c>
       <c r="O80">
         <v>1.078377302798331E-2</v>
@@ -10327,15 +10327,15 @@
       </c>
       <c r="AD80">
         <f t="shared" si="34"/>
-        <v>0.72238298223743602</v>
+        <v>0.72238298223743591</v>
       </c>
       <c r="AE80">
         <f t="shared" si="35"/>
-        <v>1.5161113355092304</v>
+        <v>1.5161113355092302</v>
       </c>
       <c r="AF80">
         <f t="shared" si="36"/>
-        <v>1.3536708352760984</v>
+        <v>1.3536708352760982</v>
       </c>
       <c r="AG80">
         <f t="shared" si="37"/>
@@ -10376,10 +10376,10 @@
         <v>-1</v>
       </c>
       <c r="M81">
-        <v>0.12593281778122509</v>
+        <v>0.1259328177812255</v>
       </c>
       <c r="N81">
-        <v>3.7929804957961652E-2</v>
+        <v>3.7929804957961617E-2</v>
       </c>
       <c r="O81">
         <v>1.8067800362836121E-2</v>
@@ -10435,7 +10435,7 @@
       </c>
       <c r="AD81">
         <f t="shared" si="34"/>
-        <v>0.79372835327179436</v>
+        <v>0.79372835327179414</v>
       </c>
       <c r="AE81" s="1"/>
       <c r="AF81" s="1"/>

</xml_diff>